<commit_message>
Update with xml parser sample
</commit_message>
<xml_diff>
--- a/parser_sample.xlsx
+++ b/parser_sample.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\vs_repos\ExcelParser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\git\ExcelParser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE34DDC-8C53-417B-9B34-D04E0460D6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAB810A-7BDE-4EFC-9451-0CE368525CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16680" yWindow="165" windowWidth="21660" windowHeight="13005" activeTab="3" xr2:uid="{81D828BD-ADA6-47DF-BEA9-B87AFAFC8FB0}"/>
+    <workbookView xWindow="-90" yWindow="10860" windowWidth="21660" windowHeight="13005" activeTab="4" xr2:uid="{81D828BD-ADA6-47DF-BEA9-B87AFAFC8FB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
     <sheet name="General" sheetId="2" r:id="rId2"/>
     <sheet name="Source" sheetId="3" r:id="rId3"/>
     <sheet name="Sink" sheetId="4" r:id="rId4"/>
-    <sheet name="Repeater" sheetId="5" r:id="rId5"/>
+    <sheet name="Sink DTD" sheetId="6" r:id="rId5"/>
+    <sheet name="Repeater" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="34">
   <si>
     <t>This is Sample</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -102,7 +103,74 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>New Option</t>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QMS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gaming</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11,22,33,44</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DTD1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DTD2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DTD3</t>
+  </si>
+  <si>
+    <t>DTD4</t>
+  </si>
+  <si>
+    <t>DTD5</t>
+  </si>
+  <si>
+    <t>DTD_V1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DTD_V2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DTD_V3</t>
+  </si>
+  <si>
+    <t>DTD_V4</t>
+  </si>
+  <si>
+    <t>4,5,6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11,22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>32,33</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CAT_Formats</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101,102</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -135,12 +203,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -149,8 +232,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -526,10 +618,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FAD5C0A-1765-4DCB-9131-94317585EF4E}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -538,117 +630,206 @@
     <col min="2" max="4" width="14.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="b">
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
         <v>0</v>
       </c>
-      <c r="C7" t="b">
+      <c r="C8" s="1">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
         <v>1</v>
       </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1">
         <v>3</v>
       </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
         <v>13</v>
       </c>
-      <c r="B11" t="b">
-        <v>0</v>
-      </c>
-      <c r="C11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -658,6 +839,226 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C8A0EE-183B-4AA0-BDE8-A8A07FCF01A7}">
+  <dimension ref="A4:M11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1">
+        <v>8</v>
+      </c>
+      <c r="G6" s="1">
+        <v>12</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>51</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>52</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>53</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2A870C-C53B-4D72-ADF8-6666DB621B30}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>